<commit_message>
Save files and add a fifth reporting column
</commit_message>
<xml_diff>
--- a/docs/Tables/Lung/Lung_2023-11-13.xlsx
+++ b/docs/Tables/Lung/Lung_2023-11-13.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Table_AS" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Table_CT" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Table_CT_AS" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Table_AS_2023-11-13" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Table_CT_2023-11-13" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Table_AS-CT_2023-11-13" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,11 @@
           <t>s</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>reporting</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -478,6 +483,11 @@
           <t>UBERON:0004884</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1. 'subsegmental bronchus' --&gt; 'lobar bronchus mesenchyme'</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -500,6 +510,11 @@
           <t>UBERON:8600000</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2. 'primary bronchiole' --&gt; 'lobular bronchiole'</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -522,6 +537,11 @@
           <t>UBERON:0002405</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3. 'lung' --&gt; 'immune system'</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -544,6 +564,11 @@
           <t>UBERON:0002299</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>4. 'respiratory bronchiole' --&gt; 'alveolus of lung'</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -566,6 +591,11 @@
           <t>UBERON:0002051</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5. 'lobular bronchiole' --&gt; 'epithelium of bronchiole'</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -588,6 +618,11 @@
           <t>UBERON:0002009</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>6. 'tracheobronchial tree' --&gt; 'pulmonary nerve plexus'</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -610,6 +645,11 @@
           <t>UBERON:8600013</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>7. 'bronchus submucosal gland' --&gt; 'submucosal gland collecting duct'</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -632,6 +672,11 @@
           <t>UBERON:8600012</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>8. 'bronchus submucosal gland' --&gt; 'submucosal gland acinus'</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -654,6 +699,11 @@
           <t>UBERON:8600013</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>9. 'bronchial submucosal gland' --&gt; 'submucosal gland collecting duct'</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -676,6 +726,11 @@
           <t>UBERON:8600012</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10. 'bronchial submucosal gland' --&gt; 'submucosal gland acinus'</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -698,6 +753,11 @@
           <t>UBERON:0004884</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>11. 'segmental bronchus' --&gt; 'lobar bronchus mesenchyme'</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -720,6 +780,11 @@
           <t>UBERON:8600017</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12. 'tracheobronchial tree' --&gt; 'bronchopulmonary segment'</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -742,6 +807,11 @@
           <t>UBERON:0002341</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>13. 'subsegmental bronchus' --&gt; 'epithelium of segmental bronchus'</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -764,6 +834,11 @@
           <t>UBERON:0012067</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>14. 'subsegmental bronchus' --&gt; 'primary bronchiole'</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -786,6 +861,11 @@
           <t>UBERON:0004515</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>15. 'lobular bronchiole' --&gt; 'smooth muscle tissue of bronchiole'</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -808,6 +888,11 @@
           <t>UBERON:0016405</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>16. 'alveolus of lung' --&gt; 'pulmonary capillary'</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -830,6 +915,11 @@
           <t>UBERON:0002173</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>17. 'respiratory bronchiole' --&gt; 'pulmonary alveolar duct'</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -852,6 +942,11 @@
           <t>UBERON:0016405</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>18. 'pulmonary alveolar duct' --&gt; 'pulmonary capillary'</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -874,6 +969,11 @@
           <t>UBERON:0016405</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>19. 'pulmonary alveolar parenchyma' --&gt; 'pulmonary capillary'</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -896,6 +996,11 @@
           <t>UBERON:0004849</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>20. 'intersegmental pulmonary vein' --&gt; 'respiratory system venous endothelium'</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -918,6 +1023,11 @@
           <t>UBERON:0004848</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>21. 'pulmonary artery' --&gt; 'respiratory system arterial endothelium'</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -940,6 +1050,11 @@
           <t>UBERON:0012416</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>22. 'pulmonary artery' --&gt; 'respiratory system arterial smooth muscle'</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -962,6 +1077,11 @@
           <t>UBERON:0004849</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>23. 'pulmonary vein' --&gt; 'respiratory system venous endothelium'</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -984,6 +1104,11 @@
           <t>UBERON:0012418</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>24. 'pulmonary vein' --&gt; 'respiratory system venous smooth muscle'</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1006,6 +1131,11 @@
           <t>UBERON:0004849</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>25. 'bronchial vein' --&gt; 'respiratory system venous endothelium'</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1026,6 +1156,11 @@
       <c r="D27" t="inlineStr">
         <is>
           <t>UBERON:0012418</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>26. 'bronchial vein' --&gt; 'respiratory system venous smooth muscle'</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1216,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1110,6 +1245,11 @@
           <t>s</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>reporting</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1132,6 +1272,11 @@
           <t>CL:0019018</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1. 'respiratory system venous smooth muscle' --&gt; 'blood vessel smooth muscle cell'</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1154,6 +1299,11 @@
           <t>CL:0019018</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2. 'respiratory system arterial smooth muscle' --&gt; 'blood vessel smooth muscle cell'</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1176,6 +1326,11 @@
           <t>CL:1000413</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3. 'respiratory system arterial endothelium' --&gt; 'endothelial cell of artery'</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1198,6 +1353,11 @@
           <t>CL:0002619</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>4. 'respiratory system venous endothelium' --&gt; 'adult endothelial progenitor cell'</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1220,6 +1380,11 @@
           <t>CL:0019003</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5. 'epithelium of segmental bronchus' --&gt; 'tracheobronchial goblet cell'</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1242,6 +1407,11 @@
           <t>CL:0002063</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>6. 'pulmonary alveolar duct' --&gt; 'type II pneumocyte'</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1264,6 +1434,11 @@
           <t>CL:4033055</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>7. 'bronchial submucosal gland ciliated duct' --&gt; 'airway submucosal gland duct ciliated cell'</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1286,6 +1461,11 @@
           <t>CL:4033024</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>8. 'submucosal gland collecting duct' --&gt; 'airway submucosal gland duct basal cell'</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1308,6 +1488,11 @@
           <t>CL:4033023</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>9. 'submucosal gland collecting duct' --&gt; 'airway submucosal gland collecting duct epithelial cell'</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1330,6 +1515,11 @@
           <t>CL:4033005</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10. 'submucosal gland acinus' --&gt; 'serous secreting cell of bronchus submucosal gland'</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1352,6 +1542,11 @@
           <t>CL:4033022</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>11. 'submucosal gland acinus' --&gt; 'mucus secreting cell of bronchus submucosal gland'</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1374,6 +1569,11 @@
           <t>CL:4033003</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12. 'submucosal gland acinus' --&gt; 'myoepithelial cell of bronchus submucosal gland'</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1396,6 +1596,11 @@
           <t>CL:4033026</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>13. 'cartilage of bronchus' --&gt; 'lung perichondrial fibroblast'</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1418,6 +1623,11 @@
           <t>CL:4033044</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>14. 'epithelium of lobar bronchus' --&gt; 'deuterosomal cell'</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1440,6 +1650,11 @@
           <t>CL:4033048</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>15. 'epithelium of lobar bronchus' --&gt; 'respiratory suprabasal cell'</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1462,6 +1677,11 @@
           <t>CL:4033055</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>16. 'ciliated ducts of bronchial submucosal gland' --&gt; 'airway submucosal gland duct ciliated cell'</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1484,6 +1704,11 @@
           <t>CL:4033048</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>17. 'epithelium of segmental bronchus' --&gt; 'respiratory suprabasal cell'</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1506,6 +1731,11 @@
           <t>CL:4033044</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>18. 'epithelium of segmental bronchus' --&gt; 'deuterosomal cell'</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1528,6 +1758,11 @@
           <t>CL:0009089</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>19. 'alveolus of lung' --&gt; 'lung pericyte'</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1550,6 +1785,11 @@
           <t>CL:0002062</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>20. 'pulmonary alveolar duct' --&gt; 'type I pneumocyte'</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1572,6 +1812,11 @@
           <t>CL:0009089</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>21. 'pulmonary alveolar duct' --&gt; 'lung pericyte'</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1594,6 +1839,11 @@
           <t>CL:4028006</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>22. 'pulmonary alveolar duct' --&gt; 'alveolar type 2 fibroblast cell'</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1616,6 +1866,11 @@
           <t>CL:4028004</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>23. 'pulmonary alveolar duct' --&gt; 'alveolar type 1 fibroblast cell'</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1638,6 +1893,11 @@
           <t>CL:4028006</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>24. 'pulmonary alveolar parenchyma' --&gt; 'alveolar type 2 fibroblast cell'</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1660,6 +1920,11 @@
           <t>CL:4028004</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>25. 'pulmonary alveolar parenchyma' --&gt; 'alveolar type 1 fibroblast cell'</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1682,6 +1947,11 @@
           <t>CL:4033008</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>26. 'respiratory system venous endothelium' --&gt; 'vein endothelial cell of respiratory system'</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1704,6 +1974,11 @@
           <t>CL:1001568</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>27. 'respiratory system arterial endothelium' --&gt; 'pulmonary artery endothelial cell'</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1724,6 +1999,11 @@
       <c r="D29" t="inlineStr">
         <is>
           <t>CL:0002591</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>28. 'respiratory system arterial smooth muscle' --&gt; 'smooth muscle cell of the pulmonary artery'</t>
         </is>
       </c>
     </row>

</xml_diff>